<commit_message>
Initial Commit of 144 Fall 2023
</commit_message>
<xml_diff>
--- a/144F20/Topic 1/test.xlsx
+++ b/144F20/Topic 1/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="14_{5F5EBD08-3467-46B8-89E6-E688C6430526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12A7878D-B456-4FBC-AA76-83C16E04A7B0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{86EF1C24-D0FB-4491-83C4-CA278CDE7181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="312" yWindow="312" windowWidth="17280" windowHeight="9204" xr2:uid="{B059B3D9-69CB-43B5-B54F-5056016079A7}"/>
   </bookViews>
@@ -446,9 +446,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" indent="1"/>
       <protection hidden="1"/>
@@ -572,6 +569,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,8 +723,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0EF9C3E4-812D-4503-859A-76D0A53D7DE2}">
-  <header guid="{0EF9C3E4-812D-4503-859A-76D0A53D7DE2}" dateTime="2023-08-25T10:09:42" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FCD0E860-103E-44EE-9CC9-D4C75DCD5833}">
+  <header guid="{FCD0E860-103E-44EE-9CC9-D4C75DCD5833}" dateTime="2023-08-31T17:17:20" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -739,7 +739,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{0EF9C3E4-812D-4503-859A-76D0A53D7DE2}" name="Richard Ketchersid" id="-1739547768" dateTime="2023-08-25T10:09:42"/>
+  <userInfo guid="{FCD0E860-103E-44EE-9CC9-D4C75DCD5833}" name="Richard Ketchersid" id="-1739563332" dateTime="2023-08-31T17:17:20"/>
 </users>
 </file>
 
@@ -1043,7 +1043,7 @@
   <dimension ref="B1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,85 +1054,85 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="30"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F5" s="34"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="36"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="4"/>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="4"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="2" t="str">
         <f ca="1">INFO("RELEASE")</f>
         <v>16.0</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="2" t="str">
         <f ca="1">INFO("SYSTEM")</f>
         <v>pcdos</v>
@@ -1140,32 +1140,32 @@
     </row>
     <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C13" s="9" t="str">
+      <c r="C13" s="8" t="str">
         <f ca="1">Sheet1!A2</f>
         <v>Your system looks good!</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
       <c r="K15" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8vSYk10RVPj7qeibvvBCnPTE9460swx1EzVe7Rr1T75Ax/JwYorCqtw75LjiXwpgN9fG+GdaDKCPVEMyMMuq3Q==" saltValue="YNSl5lvMOH50IV65L6VQvw==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FHNmH3TpI5fEXQG6gBmhVfVTsmOnzO8cdf5CU60oQsuyDqxVY3B+nPO2exGiworh1FMQUCM3D0ZbgObpGcMHYQ==" saltValue="kH9Qg9kWU7NfFMll2wo9sg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <customSheetViews>
     <customSheetView guid="{BEACEF35-7F15-4A23-9541-5B70EC08CBDC}">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D7" sqref="D7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -1249,6 +1249,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002FC4D7A32A34E94B953742578E0D227D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74d5d433463613ed438f5c69d02acddb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="d8c16f6f-632d-4fa9-9000-4a0cb55aa11b" xmlns:ns4="6588c10b-b5ed-4e95-9d69-08b9b2ce7055" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="236836fe325cd702c7dfc1167bee4fca" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1494,25 +1512,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C190D257-67B2-4C8E-9431-FB056E46BA28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A476A232-D581-47C7-B641-3FE381C85E25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5525EBA8-3762-4CFA-BB48-9EDB60D566EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1530,22 +1548,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A476A232-D581-47C7-B641-3FE381C85E25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C190D257-67B2-4C8E-9431-FB056E46BA28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>